<commit_message>
Deploying to gh-pages from  @ 098f3feb803aad08e3c663ba8a447593bd6f3520 🚀
</commit_message>
<xml_diff>
--- a/en/downloads/data-excel/16.9.1.xlsx
+++ b/en/downloads/data-excel/16.9.1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="126">
   <si>
     <t>Көрсөткүчтөрдүн аталышы</t>
   </si>
@@ -68,15 +68,6 @@
     <t>16.9.1 Доля детей в возрасте до пяти лет, рождение которых было зарегистрировано в гражданских органах, в разбивке по возрасту</t>
   </si>
   <si>
-    <t xml:space="preserve"> Көп көрсөткүчтүү кластердик изилдөөнүн маалыматтары боюнча, 2018-ж.</t>
-  </si>
-  <si>
-    <t>По данным кластерного обследования по многим показателям, 2018г.</t>
-  </si>
-  <si>
-    <t>According to the cluster survey in many respects, 2018.</t>
-  </si>
-  <si>
     <t>16.9.1 Proportion of children under 5 years of age whose births have been registered with a civil authority, by age</t>
   </si>
   <si>
@@ -203,21 +194,6 @@
     <t>No information</t>
   </si>
   <si>
-    <t>poorest</t>
-  </si>
-  <si>
-    <t>second</t>
-  </si>
-  <si>
-    <t>average</t>
-  </si>
-  <si>
-    <t>fourth</t>
-  </si>
-  <si>
-    <t>the richest</t>
-  </si>
-  <si>
     <t>Wealth quintile</t>
   </si>
   <si>
@@ -396,6 +372,36 @@
   </si>
   <si>
     <t>По возрасту (в месяцах)</t>
+  </si>
+  <si>
+    <t>(68,6)</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Көп көрсөткүчтүү кластердик изилдөөнүн маалыматтары боюнча, 2014-ж., 2018-ж., 2023-ж.</t>
+  </si>
+  <si>
+    <t>По данным кластерного обследования по многим показателям, 2014г., 2018г., 2023г.</t>
+  </si>
+  <si>
+    <t>According to Multiple Indicator Cluster Survey, 2014, 2018, 2023.</t>
+  </si>
+  <si>
+    <t>Poorest</t>
+  </si>
+  <si>
+    <t>Second</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Fourth</t>
+  </si>
+  <si>
+    <t>The richest</t>
   </si>
 </sst>
 </file>
@@ -481,19 +487,20 @@
       <charset val="204"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-      <charset val="204"/>
-    </font>
-    <font>
       <b/>
       <i/>
       <sz val="9"/>
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="204"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -561,7 +568,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -622,9 +629,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -637,8 +641,18 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -923,29 +937,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D49"/>
+  <dimension ref="A1:F49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="44.28515625" customWidth="1"/>
-    <col min="2" max="2" width="46.28515625" customWidth="1"/>
-    <col min="3" max="3" width="45.85546875" customWidth="1"/>
+    <col min="1" max="3" width="43.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
@@ -957,13 +969,13 @@
       </c>
       <c r="D2" s="12"/>
     </row>
-    <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
       <c r="D3" s="2"/>
     </row>
-    <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>0</v>
       </c>
@@ -974,12 +986,18 @@
         <v>2</v>
       </c>
       <c r="D4" s="9">
+        <v>2014</v>
+      </c>
+      <c r="E4" s="9">
         <v>2018</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F4" s="9">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="B5" s="18" t="s">
         <v>6</v>
@@ -988,240 +1006,332 @@
         <v>12</v>
       </c>
       <c r="D5" s="19">
+        <v>97.7</v>
+      </c>
+      <c r="E5" s="19">
         <v>98.9</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F5" s="19">
+        <v>99.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="D7" s="13">
+        <v>97.6</v>
+      </c>
+      <c r="E7" s="13">
+        <v>99.5</v>
+      </c>
+      <c r="F7" s="13">
+        <v>99.2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="D8" s="13">
+        <v>97.9</v>
+      </c>
+      <c r="E8" s="13">
+        <v>98.4</v>
+      </c>
+      <c r="F8" s="13">
+        <v>99.9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="33" t="s">
+        <v>61</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" s="13">
+        <v>98.5</v>
+      </c>
+      <c r="E10" s="13">
+        <v>99.1</v>
+      </c>
+      <c r="F10" s="13">
+        <v>99.3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="33" t="s">
+        <v>62</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" s="13">
+        <v>97.4</v>
+      </c>
+      <c r="E11" s="13">
+        <v>98.9</v>
+      </c>
+      <c r="F11" s="13">
+        <v>99.6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="C13" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="13">
+        <v>99.4</v>
+      </c>
+      <c r="E13" s="13">
+        <v>99.7</v>
+      </c>
+      <c r="F13" s="13">
+        <v>99.8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="C14" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" s="13">
+        <v>98.7</v>
+      </c>
+      <c r="E14" s="13">
+        <v>99.4</v>
+      </c>
+      <c r="F14" s="13">
+        <v>99.3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="C15" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" s="13">
+        <v>97.1</v>
+      </c>
+      <c r="E15" s="13">
+        <v>99.8</v>
+      </c>
+      <c r="F15" s="13">
+        <v>99.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="B6" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="C6" s="14" t="s">
-        <v>107</v>
-      </c>
-      <c r="D6" s="10"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
-        <v>120</v>
-      </c>
-      <c r="B7" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>116</v>
-      </c>
-      <c r="D7" s="13">
+      <c r="B16" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="C16" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" s="13">
+        <v>99.6</v>
+      </c>
+      <c r="E16" s="13">
+        <v>99.3</v>
+      </c>
+      <c r="F16" s="13">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="28" t="s">
+        <v>68</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="C17" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" s="13">
+        <v>95.9</v>
+      </c>
+      <c r="E17" s="13">
+        <v>99.3</v>
+      </c>
+      <c r="F17" s="13">
         <v>99.5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
-        <v>121</v>
-      </c>
-      <c r="B8" s="13" t="s">
-        <v>119</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>117</v>
-      </c>
-      <c r="D8" s="13">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="C18" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="D18" s="13">
+        <v>97</v>
+      </c>
+      <c r="E18" s="13">
+        <v>99.5</v>
+      </c>
+      <c r="F18" s="13">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="C19" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="D19" s="13">
+        <v>97.4</v>
+      </c>
+      <c r="E19" s="13">
+        <v>96.8</v>
+      </c>
+      <c r="F19" s="13">
+        <v>99.4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="D20" s="13">
         <v>98.4</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="27" t="s">
-        <v>68</v>
-      </c>
-      <c r="B9" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="D9" s="13"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="28" t="s">
-        <v>69</v>
-      </c>
-      <c r="B10" s="13" t="s">
+      <c r="E20" s="13">
+        <v>99.2</v>
+      </c>
+      <c r="F20" s="13">
+        <v>99.3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="B21" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="D10" s="13">
-        <v>99.1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="28" t="s">
-        <v>70</v>
-      </c>
-      <c r="B11" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="D11" s="13">
-        <v>98.9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="27" t="s">
-        <v>71</v>
-      </c>
-      <c r="B12" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="C12" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="D12" s="13"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="29" t="s">
-        <v>72</v>
-      </c>
-      <c r="B13" s="13" t="s">
+      <c r="C21" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="D21" s="13">
+        <v>98.8</v>
+      </c>
+      <c r="E21" s="13">
+        <v>97.5</v>
+      </c>
+      <c r="F21" s="13">
         <v>100</v>
       </c>
-      <c r="C13" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="D13" s="13">
-        <v>99.7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="29" t="s">
-        <v>73</v>
-      </c>
-      <c r="B14" s="13" t="s">
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="C22" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="C14" s="24" t="s">
-        <v>46</v>
-      </c>
-      <c r="D14" s="13">
-        <v>99.4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="29" t="s">
-        <v>74</v>
-      </c>
-      <c r="B15" s="13" t="s">
-        <v>102</v>
-      </c>
-      <c r="C15" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="D15" s="13">
-        <v>99.8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="29" t="s">
-        <v>75</v>
-      </c>
-      <c r="B16" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="C16" s="24" t="s">
-        <v>48</v>
-      </c>
-      <c r="D16" s="13">
-        <v>99.3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="29" t="s">
-        <v>76</v>
-      </c>
-      <c r="B17" s="13" t="s">
-        <v>104</v>
-      </c>
-      <c r="C17" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="D17" s="13">
-        <v>99.3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="29" t="s">
-        <v>77</v>
-      </c>
-      <c r="B18" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="C18" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="D18" s="13">
-        <v>99.5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="29" t="s">
-        <v>78</v>
-      </c>
-      <c r="B19" s="13" t="s">
-        <v>106</v>
-      </c>
-      <c r="C19" s="24" t="s">
-        <v>51</v>
-      </c>
-      <c r="D19" s="13">
-        <v>96.8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="30" t="s">
-        <v>79</v>
-      </c>
-      <c r="B20" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="C20" s="24" t="s">
-        <v>52</v>
-      </c>
-      <c r="D20" s="13">
-        <v>99.2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="30" t="s">
-        <v>80</v>
-      </c>
-      <c r="B21" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="C21" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="D21" s="13">
-        <v>97.5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="15" t="s">
-        <v>122</v>
-      </c>
-      <c r="B22" s="15" t="s">
-        <v>123</v>
-      </c>
-      <c r="C22" s="15" t="s">
-        <v>109</v>
-      </c>
       <c r="D22" s="13"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
         <v>7</v>
       </c>
@@ -1232,10 +1342,16 @@
         <v>7</v>
       </c>
       <c r="D23" s="13">
+        <v>95.4</v>
+      </c>
+      <c r="E23" s="13">
         <v>96.9</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F23" s="13">
+        <v>98.4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="20" t="s">
         <v>11</v>
       </c>
@@ -1246,10 +1362,16 @@
         <v>11</v>
       </c>
       <c r="D24" s="13">
+        <v>96</v>
+      </c>
+      <c r="E24" s="13">
         <v>98.8</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F24" s="13">
+        <v>99.7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
         <v>8</v>
       </c>
@@ -1260,10 +1382,16 @@
         <v>8</v>
       </c>
       <c r="D25" s="13">
+        <v>98.8</v>
+      </c>
+      <c r="E25" s="13">
         <v>99.2</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F25" s="13">
+        <v>99.7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
         <v>9</v>
       </c>
@@ -1274,10 +1402,16 @@
         <v>9</v>
       </c>
       <c r="D26" s="13">
+        <v>97.6</v>
+      </c>
+      <c r="E26" s="13">
         <v>99.9</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F26" s="13">
+        <v>99.7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
         <v>10</v>
       </c>
@@ -1288,279 +1422,386 @@
         <v>10</v>
       </c>
       <c r="D27" s="13">
+        <v>98.7</v>
+      </c>
+      <c r="E27" s="13">
         <v>99.8</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F27" s="13">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="B28" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C28" s="25" t="s">
+        <v>102</v>
+      </c>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="33" t="s">
+        <v>74</v>
+      </c>
+      <c r="B29" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C29" s="23" t="s">
+        <v>103</v>
+      </c>
+      <c r="D29" s="21" t="s">
+        <v>116</v>
+      </c>
+      <c r="E29" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="F29" s="21" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="33" t="s">
+        <v>75</v>
+      </c>
+      <c r="B30" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C30" s="23" t="s">
+        <v>104</v>
+      </c>
+      <c r="D30" s="13">
+        <v>96.4</v>
+      </c>
+      <c r="E30" s="13">
+        <v>98.1</v>
+      </c>
+      <c r="F30" s="13">
+        <v>98.7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="B31" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C31" s="23" t="s">
+        <v>105</v>
+      </c>
+      <c r="D31" s="13">
+        <v>97.8</v>
+      </c>
+      <c r="E31" s="13">
+        <v>98.8</v>
+      </c>
+      <c r="F31" s="13">
+        <v>99.6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="33" t="s">
+        <v>76</v>
+      </c>
+      <c r="B32" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C32" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="D32" s="13">
+        <v>99.1</v>
+      </c>
+      <c r="E32" s="13">
+        <v>98.8</v>
+      </c>
+      <c r="F32" s="13">
+        <v>99.6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="33" t="s">
+        <v>77</v>
+      </c>
+      <c r="B33" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C33" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="D33" s="13">
+        <v>98.7</v>
+      </c>
+      <c r="E33" s="13">
+        <v>99.5</v>
+      </c>
+      <c r="F33" s="13">
+        <v>99.7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="32" t="s">
+        <v>90</v>
+      </c>
+      <c r="B34" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="C34" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="B35" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C35" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="D35" s="21" t="s">
+        <v>117</v>
+      </c>
+      <c r="E35" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="F35" s="21">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="B36" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C36" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="D36" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="E36" s="13">
+        <v>99.6</v>
+      </c>
+      <c r="F36" s="13">
+        <v>99.8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="32" t="s">
+        <v>91</v>
+      </c>
+      <c r="B37" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C37" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="D37" s="35"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="B38" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C38" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="D38" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="E38" s="13">
+        <v>97.7</v>
+      </c>
+      <c r="F38" s="35" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="B39" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C39" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="D39" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="E39" s="13">
+        <v>98.9</v>
+      </c>
+      <c r="F39" s="13">
+        <v>99.5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="B40" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C40" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="D40" s="36" t="s">
+        <v>117</v>
+      </c>
+      <c r="E40" s="22">
+        <v>100</v>
+      </c>
+      <c r="F40" s="36" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="B41" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C41" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="D41" s="13"/>
+      <c r="E41" s="13"/>
+      <c r="F41" s="13"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="30" t="s">
         <v>81</v>
       </c>
-      <c r="B28" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="C28" s="25" t="s">
-        <v>110</v>
-      </c>
-      <c r="D28" s="13"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="28" t="s">
+      <c r="B42" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C42" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="D42" s="22">
+        <v>95.8</v>
+      </c>
+      <c r="E42" s="22">
+        <v>99</v>
+      </c>
+      <c r="F42" s="22">
+        <v>99.3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="30" t="s">
         <v>82</v>
       </c>
-      <c r="B29" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="C29" s="23" t="s">
-        <v>111</v>
-      </c>
-      <c r="D29" s="21" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="28" t="s">
+      <c r="B43" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C43" s="23" t="s">
+        <v>122</v>
+      </c>
+      <c r="D43" s="13">
+        <v>97.8</v>
+      </c>
+      <c r="E43" s="13">
+        <v>98.4</v>
+      </c>
+      <c r="F43" s="13">
+        <v>99.2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="30" t="s">
         <v>83</v>
       </c>
-      <c r="B30" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="C30" s="23" t="s">
-        <v>112</v>
-      </c>
-      <c r="D30" s="13">
-        <v>98.1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="28" t="s">
-        <v>96</v>
-      </c>
-      <c r="B31" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="C31" s="23" t="s">
-        <v>113</v>
-      </c>
-      <c r="D31" s="13">
+      <c r="B44" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C44" s="23" t="s">
+        <v>123</v>
+      </c>
+      <c r="D44" s="13">
+        <v>98.3</v>
+      </c>
+      <c r="E44" s="13">
         <v>98.8</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="28" t="s">
+      <c r="F44" s="13">
+        <v>99.7</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="30" t="s">
         <v>84</v>
       </c>
-      <c r="B32" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="C32" s="23" t="s">
-        <v>114</v>
-      </c>
-      <c r="D32" s="13">
-        <v>98.8</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="28" t="s">
+      <c r="B45" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C45" s="23" t="s">
+        <v>124</v>
+      </c>
+      <c r="D45" s="13">
+        <v>98</v>
+      </c>
+      <c r="E45" s="13">
+        <v>99.1</v>
+      </c>
+      <c r="F45" s="13">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="31" t="s">
         <v>85</v>
       </c>
-      <c r="B33" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="C33" s="23" t="s">
-        <v>115</v>
-      </c>
-      <c r="D33" s="13">
-        <v>99.5</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="33" t="s">
-        <v>98</v>
-      </c>
-      <c r="B34" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="C34" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="D34" s="13"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="B35" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="C35" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="D35" s="21" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="B36" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="C36" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="D36" s="13">
+      <c r="B46" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C46" s="26" t="s">
+        <v>125</v>
+      </c>
+      <c r="D46" s="16">
+        <v>99.1</v>
+      </c>
+      <c r="E46" s="16">
         <v>99.6</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="33" t="s">
-        <v>99</v>
-      </c>
-      <c r="B37" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="C37" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="D37" s="13"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="B38" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="C38" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="D38" s="13">
-        <v>97.7</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="B39" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="C39" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="D39" s="13">
-        <v>98.9</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="B40" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="C40" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="D40" s="22">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="25" t="s">
-        <v>97</v>
-      </c>
-      <c r="B41" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="C41" s="25" t="s">
-        <v>64</v>
-      </c>
-      <c r="D41" s="13"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="31" t="s">
-        <v>89</v>
-      </c>
-      <c r="B42" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="C42" s="23" t="s">
-        <v>59</v>
-      </c>
-      <c r="D42" s="22">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="31" t="s">
-        <v>90</v>
-      </c>
-      <c r="B43" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="C43" s="23" t="s">
-        <v>60</v>
-      </c>
-      <c r="D43" s="13">
-        <v>98.4</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="31" t="s">
-        <v>91</v>
-      </c>
-      <c r="B44" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="C44" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="D44" s="13">
-        <v>98.8</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="31" t="s">
-        <v>92</v>
-      </c>
-      <c r="B45" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="C45" s="23" t="s">
-        <v>62</v>
-      </c>
-      <c r="D45" s="13">
-        <v>99.1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="32" t="s">
-        <v>93</v>
-      </c>
-      <c r="B46" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="C46" s="26" t="s">
-        <v>63</v>
-      </c>
-      <c r="D46" s="16">
+      <c r="F46" s="16">
         <v>99.6</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
-        <v>14</v>
+        <v>118</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>15</v>
+        <v>119</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+      <c r="D47" s="34"/>
+      <c r="E47" s="34"/>
+      <c r="F47" s="34"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="13"/>
       <c r="B48" s="13"/>
       <c r="C48" s="13"/>

</xml_diff>